<commit_message>
Optimised file path for extent reports
</commit_message>
<xml_diff>
--- a/Framework/TestData/Data.xlsx
+++ b/Framework/TestData/Data.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SignUpData" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,9 +21,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">anmol@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gupta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InstaCEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anmol29@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -104,7 +117,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -115,6 +128,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -136,7 +153,7 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -166,4 +183,54 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>12345678</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1" display="anmol29@yopmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Seperated and created new file test case for login with wrong credential
</commit_message>
<xml_diff>
--- a/Framework/TestData/Data.xlsx
+++ b/Framework/TestData/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,9 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">anmol@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filty@yomail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Anmol</t>
@@ -151,10 +154,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -171,9 +174,18 @@
         <v>12345678</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>12345678</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="anmol@yopmail.com"/>
+    <hyperlink ref="A2" r:id="rId2" display="filty@yomail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -192,7 +204,7 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -203,16 +215,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>12345678</v>

</xml_diff>

<commit_message>
Sign Up Test Case completion along with reports and snapshots.
</commit_message>
<xml_diff>
--- a/Framework/TestData/Data.xlsx
+++ b/Framework/TestData/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
     <t xml:space="preserve">InstaCEI</t>
   </si>
   <si>
-    <t xml:space="preserve">anmol29@yopmail.com</t>
+    <t xml:space="preserve">anmol111@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -156,7 +156,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -204,8 +204,8 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -213,7 +213,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>2</v>
       </c>
@@ -234,9 +234,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" display="anmol29@yopmail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Excel Sheet updation, Home page element updation and test reports
</commit_message>
<xml_diff>
--- a/Framework/TestData/Data.xlsx
+++ b/Framework/TestData/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -156,8 +156,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -166,7 +166,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -204,7 +204,7 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>